<commit_message>
Add screencast of working version (st 0.83.0)
</commit_message>
<xml_diff>
--- a/parms.xlsx
+++ b/parms.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F75FF30A-9070-4A52-98F3-F279A25B5B74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{373EFD87-4967-4125-8B87-4D2A3B820A88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{2526FB6E-82DB-4BB3-81DF-77C2972D279F}"/>
   </bookViews>
@@ -861,10 +861,10 @@
   <dimension ref="A1:U20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C20" sqref="C20"/>
+      <selection pane="bottomRight" activeCell="U19" sqref="U19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1296,7 +1296,7 @@
         <v>Tiger?</v>
       </c>
       <c r="U6" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.45">
@@ -1911,7 +1911,7 @@
         <v>Elephant?</v>
       </c>
       <c r="U15" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.45">
@@ -2117,7 +2117,7 @@
         <v>Koala?</v>
       </c>
       <c r="U18" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.45">

</xml_diff>